<commit_message>
adds part3 to DHS
</commit_message>
<xml_diff>
--- a/programs/addtoWIDE_countries.xlsx
+++ b/programs/addtoWIDE_countries.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rosa_V\Dropbox\WIDE\WIDE\programs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F714181D-A336-411E-8E45-0B41E9B659FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0073767F-7FB2-4AC4-AEB4-4C7804660A43}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="650" yWindow="760" windowWidth="17640" windowHeight="8930" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="680" yWindow="270" windowWidth="17640" windowHeight="8930" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="surveys to include" sheetId="7" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6754" uniqueCount="569">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6754" uniqueCount="570">
   <si>
     <t>iso_code3</t>
   </si>
@@ -1699,12 +1699,6 @@
     <t>PK</t>
   </si>
   <si>
-    <t>Be careful with this because it was already in "Part1" as Benin/2017</t>
-  </si>
-  <si>
-    <t>Be careful with this because it was already in "Part2" as Nigeria/2018</t>
-  </si>
-  <si>
     <t>a</t>
   </si>
   <si>
@@ -1748,6 +1742,16 @@
   </si>
   <si>
     <t>MICS6</t>
+  </si>
+  <si>
+    <t>Be careful with this because it was already in "Part1" as Benin_2017</t>
+  </si>
+  <si>
+    <t>Be careful with this because it was already in "Part2" as Nigeria_2018</t>
+  </si>
+  <si>
+    <t>iso_
+code3</t>
   </si>
 </sst>
 </file>
@@ -2118,7 +2122,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="129">
+  <cellXfs count="131">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2344,76 +2348,11 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2450,6 +2389,81 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -2736,1004 +2750,937 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J4" sqref="J4"/>
+      <selection pane="bottomLeft" sqref="A1:E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.6328125" style="103" customWidth="1"/>
-    <col min="2" max="2" width="7.453125" style="103" customWidth="1"/>
-    <col min="3" max="3" width="5.08984375" style="103" customWidth="1"/>
-    <col min="4" max="4" width="16.7265625" style="103" customWidth="1"/>
-    <col min="5" max="5" width="8.7265625" style="84"/>
-    <col min="6" max="6" width="19.6328125" style="103" customWidth="1"/>
-    <col min="7" max="7" width="12.36328125" style="103" customWidth="1"/>
-    <col min="8" max="8" width="13" style="103" customWidth="1"/>
-    <col min="9" max="9" width="7" style="109" customWidth="1"/>
-    <col min="10" max="10" width="19" style="109" customWidth="1"/>
-    <col min="11" max="16384" width="8.7265625" style="103"/>
+    <col min="1" max="1" width="9.36328125" style="123" customWidth="1"/>
+    <col min="2" max="2" width="7.453125" style="123" customWidth="1"/>
+    <col min="3" max="3" width="5.6328125" style="123" customWidth="1"/>
+    <col min="4" max="4" width="16.7265625" style="123" customWidth="1"/>
+    <col min="5" max="5" width="8.7265625" style="126"/>
+    <col min="6" max="6" width="19.6328125" style="123" customWidth="1"/>
+    <col min="7" max="7" width="12.36328125" style="123" customWidth="1"/>
+    <col min="8" max="8" width="13" style="123" customWidth="1"/>
+    <col min="9" max="9" width="7" style="110" customWidth="1"/>
+    <col min="10" max="10" width="19" style="110" customWidth="1"/>
+    <col min="11" max="16384" width="8.7265625" style="123"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" s="92" customFormat="1" ht="65" x14ac:dyDescent="0.35">
-      <c r="A1" s="92" t="s">
-        <v>557</v>
-      </c>
-      <c r="B1" s="93" t="s">
+    <row r="1" spans="1:45" s="101" customFormat="1" ht="65" x14ac:dyDescent="0.35">
+      <c r="A1" s="102" t="s">
+        <v>555</v>
+      </c>
+      <c r="B1" s="102" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="93" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="93" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="91" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="93" t="s">
+      <c r="C1" s="102" t="s">
+        <v>569</v>
+      </c>
+      <c r="D1" s="102" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="103" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="102" t="s">
         <v>68</v>
       </c>
-      <c r="G1" s="93" t="s">
+      <c r="G1" s="102" t="s">
         <v>67</v>
       </c>
-      <c r="H1" s="92" t="s">
+      <c r="H1" s="101" t="s">
+        <v>561</v>
+      </c>
+      <c r="I1" s="102" t="s">
+        <v>565</v>
+      </c>
+      <c r="J1" s="101" t="s">
+        <v>559</v>
+      </c>
+      <c r="K1" s="104" t="s">
+        <v>72</v>
+      </c>
+      <c r="L1" s="105" t="s">
+        <v>69</v>
+      </c>
+      <c r="M1" s="105" t="s">
+        <v>70</v>
+      </c>
+      <c r="N1" s="105" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:45" s="106" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="127" t="s">
+        <v>539</v>
+      </c>
+      <c r="B2" s="106" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="86" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="86" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="107">
+        <v>2018</v>
+      </c>
+      <c r="F2" s="86" t="s">
+        <v>63</v>
+      </c>
+      <c r="G2" s="86" t="s">
+        <v>60</v>
+      </c>
+      <c r="H2" s="108" t="s">
+        <v>567</v>
+      </c>
+      <c r="I2" s="109" t="s">
+        <v>60</v>
+      </c>
+      <c r="J2" s="110" t="s">
         <v>563</v>
       </c>
-      <c r="I1" s="93" t="s">
-        <v>567</v>
-      </c>
-      <c r="J1" s="92" t="s">
-        <v>561</v>
-      </c>
-      <c r="K1" s="94" t="s">
-        <v>72</v>
-      </c>
-      <c r="L1" s="95" t="s">
-        <v>69</v>
-      </c>
-      <c r="M1" s="95" t="s">
-        <v>70</v>
-      </c>
-      <c r="N1" s="95" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="2" spans="1:45" s="97" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="96" t="s">
+      <c r="K2" s="111">
+        <v>6</v>
+      </c>
+      <c r="L2" s="112">
+        <v>6</v>
+      </c>
+      <c r="M2" s="112">
+        <v>4</v>
+      </c>
+      <c r="N2" s="112">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:45" s="106" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="127" t="s">
         <v>539</v>
       </c>
-      <c r="B2" s="97" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="96" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="96" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="88">
+      <c r="B3" s="86" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="86" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="86" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="107">
         <v>2018</v>
       </c>
-      <c r="F2" s="96" t="s">
+      <c r="F3" s="86" t="s">
         <v>63</v>
       </c>
-      <c r="G2" s="96" t="s">
+      <c r="G3" s="86" t="s">
         <v>60</v>
       </c>
-      <c r="H2" s="98" t="s">
-        <v>552</v>
-      </c>
-      <c r="I2" s="99" t="s">
+      <c r="H3" s="86"/>
+      <c r="I3" s="109" t="s">
         <v>60</v>
       </c>
-      <c r="J2" s="109" t="s">
-        <v>565</v>
-      </c>
-      <c r="K2" s="100">
-        <v>6</v>
-      </c>
-      <c r="L2" s="90">
-        <v>6</v>
-      </c>
-      <c r="M2" s="90">
-        <v>4</v>
-      </c>
-      <c r="N2" s="90">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:45" s="97" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="96" t="s">
+      <c r="J3" s="110" t="s">
+        <v>563</v>
+      </c>
+      <c r="K3" s="111">
+        <v>7</v>
+      </c>
+      <c r="L3" s="112">
+        <v>6</v>
+      </c>
+      <c r="M3" s="112">
+        <v>4</v>
+      </c>
+      <c r="N3" s="112">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:45" s="106" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="127" t="s">
         <v>539</v>
       </c>
-      <c r="B3" s="96" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="96" t="s">
+      <c r="B4" s="86" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="86" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="86" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="107">
+        <v>2018</v>
+      </c>
+      <c r="F4" s="86" t="s">
+        <v>63</v>
+      </c>
+      <c r="G4" s="86" t="s">
+        <v>60</v>
+      </c>
+      <c r="H4" s="86"/>
+      <c r="I4" s="109" t="s">
+        <v>60</v>
+      </c>
+      <c r="J4" s="113" t="s">
+        <v>564</v>
+      </c>
+      <c r="K4" s="111">
+        <v>7</v>
+      </c>
+      <c r="L4" s="112">
+        <v>6</v>
+      </c>
+      <c r="M4" s="112">
+        <v>3</v>
+      </c>
+      <c r="N4" s="112">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:45" s="106" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="127" t="s">
+        <v>539</v>
+      </c>
+      <c r="B5" s="86" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="86" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" s="86" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" s="107">
+        <v>2018</v>
+      </c>
+      <c r="F5" s="86" t="s">
+        <v>63</v>
+      </c>
+      <c r="G5" s="86" t="s">
+        <v>60</v>
+      </c>
+      <c r="H5" s="108" t="s">
+        <v>568</v>
+      </c>
+      <c r="I5" s="109" t="s">
+        <v>60</v>
+      </c>
+      <c r="J5" s="110" t="s">
+        <v>563</v>
+      </c>
+      <c r="K5" s="111">
+        <v>6</v>
+      </c>
+      <c r="L5" s="112">
+        <v>6</v>
+      </c>
+      <c r="M5" s="112">
+        <v>3</v>
+      </c>
+      <c r="N5" s="112">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:45" s="106" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="127" t="s">
+        <v>539</v>
+      </c>
+      <c r="B6" s="86" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="86" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" s="86" t="s">
+        <v>45</v>
+      </c>
+      <c r="E6" s="107">
+        <v>2017</v>
+      </c>
+      <c r="F6" s="86" t="s">
+        <v>558</v>
+      </c>
+      <c r="G6" s="86" t="s">
+        <v>62</v>
+      </c>
+      <c r="H6" s="86"/>
+      <c r="I6" s="109" t="s">
+        <v>60</v>
+      </c>
+      <c r="J6" s="110" t="s">
+        <v>563</v>
+      </c>
+      <c r="K6" s="114">
+        <v>6</v>
+      </c>
+      <c r="L6" s="115">
+        <v>6</v>
+      </c>
+      <c r="M6" s="115">
+        <v>4</v>
+      </c>
+      <c r="N6" s="115">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:45" s="106" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="127" t="s">
+        <v>539</v>
+      </c>
+      <c r="B7" s="86" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="86" t="s">
+        <v>54</v>
+      </c>
+      <c r="D7" s="86" t="s">
+        <v>55</v>
+      </c>
+      <c r="E7" s="107">
+        <v>2016</v>
+      </c>
+      <c r="F7" s="86" t="s">
+        <v>63</v>
+      </c>
+      <c r="G7" s="86" t="s">
+        <v>61</v>
+      </c>
+      <c r="H7" s="86"/>
+      <c r="I7" s="109" t="s">
+        <v>60</v>
+      </c>
+      <c r="J7" s="110" t="s">
+        <v>563</v>
+      </c>
+      <c r="K7" s="111">
+        <v>7</v>
+      </c>
+      <c r="L7" s="112">
+        <v>7</v>
+      </c>
+      <c r="M7" s="112">
+        <v>2</v>
+      </c>
+      <c r="N7" s="112">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:45" s="106" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="127" t="s">
+        <v>539</v>
+      </c>
+      <c r="B8" s="86" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="86" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8" s="86" t="s">
+        <v>57</v>
+      </c>
+      <c r="E8" s="107">
+        <v>2018</v>
+      </c>
+      <c r="F8" s="86" t="s">
+        <v>63</v>
+      </c>
+      <c r="G8" s="86" t="s">
+        <v>60</v>
+      </c>
+      <c r="H8" s="86"/>
+      <c r="I8" s="109" t="s">
+        <v>60</v>
+      </c>
+      <c r="J8" s="110" t="s">
+        <v>563</v>
+      </c>
+      <c r="K8" s="111">
+        <v>7</v>
+      </c>
+      <c r="L8" s="112">
+        <v>7</v>
+      </c>
+      <c r="M8" s="112">
+        <v>2</v>
+      </c>
+      <c r="N8" s="112">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:45" s="106" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="128" t="s">
+        <v>554</v>
+      </c>
+      <c r="B9" s="106" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="106" t="s">
+        <v>363</v>
+      </c>
+      <c r="D9" s="106" t="s">
+        <v>364</v>
+      </c>
+      <c r="E9" s="112">
+        <v>2016</v>
+      </c>
+      <c r="F9" s="106" t="s">
+        <v>63</v>
+      </c>
+      <c r="G9" s="106" t="s">
+        <v>60</v>
+      </c>
+      <c r="I9" s="109" t="s">
+        <v>63</v>
+      </c>
+      <c r="J9" s="109"/>
+      <c r="K9" s="86"/>
+      <c r="L9" s="86"/>
+      <c r="M9" s="86"/>
+      <c r="N9" s="86"/>
+    </row>
+    <row r="10" spans="1:45" s="86" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="129" t="s">
+        <v>538</v>
+      </c>
+      <c r="B10" s="116" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="116" t="s">
+        <v>79</v>
+      </c>
+      <c r="D10" s="116" t="s">
+        <v>80</v>
+      </c>
+      <c r="E10" s="117">
+        <v>2017</v>
+      </c>
+      <c r="F10" s="106" t="s">
+        <v>63</v>
+      </c>
+      <c r="G10" s="106" t="s">
+        <v>60</v>
+      </c>
+      <c r="H10" s="106"/>
+      <c r="I10" s="109" t="s">
+        <v>63</v>
+      </c>
+      <c r="J10" s="109"/>
+    </row>
+    <row r="11" spans="1:45" s="122" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="129" t="s">
+        <v>538</v>
+      </c>
+      <c r="B11" s="116" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="116" t="s">
+        <v>235</v>
+      </c>
+      <c r="D11" s="100" t="s">
+        <v>236</v>
+      </c>
+      <c r="E11" s="118">
+        <v>2017</v>
+      </c>
+      <c r="F11" s="119" t="s">
+        <v>63</v>
+      </c>
+      <c r="G11" s="119" t="s">
+        <v>60</v>
+      </c>
+      <c r="H11" s="119"/>
+      <c r="I11" s="109" t="s">
+        <v>60</v>
+      </c>
+      <c r="J11" s="110" t="s">
+        <v>563</v>
+      </c>
+      <c r="K11" s="120">
+        <v>6</v>
+      </c>
+      <c r="L11" s="121">
+        <v>6</v>
+      </c>
+      <c r="M11" s="121">
+        <v>3</v>
+      </c>
+      <c r="N11" s="121">
+        <v>4</v>
+      </c>
+      <c r="O11" s="86"/>
+      <c r="P11" s="86"/>
+      <c r="Q11" s="86"/>
+      <c r="R11" s="86"/>
+      <c r="S11" s="86"/>
+      <c r="T11" s="86"/>
+      <c r="U11" s="86"/>
+      <c r="V11" s="86"/>
+      <c r="W11" s="86"/>
+      <c r="X11" s="86"/>
+      <c r="Y11" s="86"/>
+      <c r="Z11" s="86"/>
+      <c r="AA11" s="86"/>
+      <c r="AB11" s="86"/>
+      <c r="AC11" s="86"/>
+      <c r="AD11" s="86"/>
+      <c r="AE11" s="86"/>
+      <c r="AF11" s="86"/>
+      <c r="AG11" s="86"/>
+      <c r="AH11" s="86"/>
+      <c r="AI11" s="86"/>
+      <c r="AJ11" s="86"/>
+      <c r="AK11" s="86"/>
+      <c r="AL11" s="86"/>
+      <c r="AM11" s="86"/>
+      <c r="AN11" s="86"/>
+      <c r="AO11" s="86"/>
+      <c r="AP11" s="86"/>
+      <c r="AQ11" s="86"/>
+      <c r="AR11" s="86"/>
+      <c r="AS11" s="86"/>
+    </row>
+    <row r="12" spans="1:45" s="87" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="129" t="s">
+        <v>538</v>
+      </c>
+      <c r="B12" s="116" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="116" t="s">
+        <v>249</v>
+      </c>
+      <c r="D12" s="100" t="s">
+        <v>250</v>
+      </c>
+      <c r="E12" s="118">
+        <v>2017</v>
+      </c>
+      <c r="F12" s="119" t="s">
+        <v>63</v>
+      </c>
+      <c r="G12" s="119" t="s">
+        <v>60</v>
+      </c>
+      <c r="H12" s="119"/>
+      <c r="I12" s="109" t="s">
+        <v>60</v>
+      </c>
+      <c r="J12" s="110" t="s">
+        <v>563</v>
+      </c>
+      <c r="K12" s="120">
+        <v>7</v>
+      </c>
+      <c r="L12" s="121">
+        <v>6</v>
+      </c>
+      <c r="M12" s="121">
+        <v>3</v>
+      </c>
+      <c r="N12" s="121">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:45" s="87" customFormat="1" ht="15.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="129" t="s">
+        <v>538</v>
+      </c>
+      <c r="B13" s="116" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="116" t="s">
+        <v>301</v>
+      </c>
+      <c r="D13" s="100" t="s">
+        <v>302</v>
+      </c>
+      <c r="E13" s="118">
+        <v>2017</v>
+      </c>
+      <c r="F13" s="119" t="s">
+        <v>63</v>
+      </c>
+      <c r="G13" s="119" t="s">
+        <v>60</v>
+      </c>
+      <c r="H13" s="119"/>
+      <c r="I13" s="109" t="s">
+        <v>60</v>
+      </c>
+      <c r="J13" s="110" t="s">
+        <v>563</v>
+      </c>
+      <c r="K13" s="120">
+        <v>6</v>
+      </c>
+      <c r="L13" s="121">
+        <v>7</v>
+      </c>
+      <c r="M13" s="121">
+        <v>3</v>
+      </c>
+      <c r="N13" s="121">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:45" s="87" customFormat="1" ht="15.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="129" t="s">
+        <v>538</v>
+      </c>
+      <c r="B14" s="116" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="116" t="s">
+        <v>355</v>
+      </c>
+      <c r="D14" s="100" t="s">
+        <v>356</v>
+      </c>
+      <c r="E14" s="118">
+        <v>2018</v>
+      </c>
+      <c r="F14" s="119" t="s">
+        <v>63</v>
+      </c>
+      <c r="G14" s="119" t="s">
+        <v>60</v>
+      </c>
+      <c r="H14" s="119"/>
+      <c r="I14" s="109" t="s">
+        <v>60</v>
+      </c>
+      <c r="J14" s="113" t="s">
+        <v>564</v>
+      </c>
+      <c r="K14" s="120">
+        <v>5</v>
+      </c>
+      <c r="L14" s="121">
+        <v>5</v>
+      </c>
+      <c r="M14" s="121">
+        <v>3</v>
+      </c>
+      <c r="N14" s="121">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:45" s="87" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="129" t="s">
+        <v>538</v>
+      </c>
+      <c r="B15" s="116" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="116" t="s">
+        <v>369</v>
+      </c>
+      <c r="D15" s="100" t="s">
+        <v>370</v>
+      </c>
+      <c r="E15" s="118">
+        <v>2018</v>
+      </c>
+      <c r="F15" s="119" t="s">
+        <v>63</v>
+      </c>
+      <c r="G15" s="119" t="s">
+        <v>60</v>
+      </c>
+      <c r="H15" s="119"/>
+      <c r="I15" s="109" t="s">
+        <v>60</v>
+      </c>
+      <c r="J15" s="113" t="s">
+        <v>564</v>
+      </c>
+      <c r="K15" s="120">
+        <v>6</v>
+      </c>
+      <c r="L15" s="121">
+        <v>6</v>
+      </c>
+      <c r="M15" s="121">
+        <v>3</v>
+      </c>
+      <c r="N15" s="121">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:45" s="86" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="129" t="s">
+        <v>538</v>
+      </c>
+      <c r="B16" s="116" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="116" t="s">
+        <v>445</v>
+      </c>
+      <c r="D16" s="100" t="s">
+        <v>446</v>
+      </c>
+      <c r="E16" s="118">
+        <v>2017</v>
+      </c>
+      <c r="F16" s="119" t="s">
+        <v>63</v>
+      </c>
+      <c r="G16" s="119" t="s">
+        <v>60</v>
+      </c>
+      <c r="H16" s="119"/>
+      <c r="I16" s="109" t="s">
+        <v>60</v>
+      </c>
+      <c r="J16" s="113" t="s">
+        <v>564</v>
+      </c>
+      <c r="K16" s="120">
+        <v>7</v>
+      </c>
+      <c r="L16" s="121">
+        <v>4</v>
+      </c>
+      <c r="M16" s="121">
+        <v>5</v>
+      </c>
+      <c r="N16" s="121">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" s="86" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="127" t="s">
+        <v>539</v>
+      </c>
+      <c r="B17" s="86" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="86" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" s="86" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17" s="107">
+        <v>2015</v>
+      </c>
+      <c r="F17" s="86" t="s">
+        <v>63</v>
+      </c>
+      <c r="G17" s="86" t="s">
+        <v>66</v>
+      </c>
+      <c r="H17" s="123"/>
+      <c r="I17" s="109" t="s">
+        <v>60</v>
+      </c>
+      <c r="J17" s="109"/>
+      <c r="K17" s="111">
+        <v>6</v>
+      </c>
+      <c r="L17" s="112">
+        <v>6</v>
+      </c>
+      <c r="M17" s="112">
+        <v>4</v>
+      </c>
+      <c r="N17" s="112">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" s="87" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="127" t="s">
+        <v>539</v>
+      </c>
+      <c r="B18" s="86" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="86" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="101" t="s">
+      <c r="D18" s="86" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="88">
+      <c r="E18" s="107">
+        <v>2016</v>
+      </c>
+      <c r="F18" s="86" t="s">
+        <v>63</v>
+      </c>
+      <c r="G18" s="86" t="s">
+        <v>66</v>
+      </c>
+      <c r="H18" s="123"/>
+      <c r="I18" s="109" t="s">
+        <v>60</v>
+      </c>
+      <c r="J18" s="109"/>
+      <c r="K18" s="111">
+        <v>7</v>
+      </c>
+      <c r="L18" s="112">
+        <v>6</v>
+      </c>
+      <c r="M18" s="112">
+        <v>4</v>
+      </c>
+      <c r="N18" s="112">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A19" s="130" t="s">
+        <v>539</v>
+      </c>
+      <c r="B19" s="87" t="s">
+        <v>566</v>
+      </c>
+      <c r="C19" s="87" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" s="87" t="s">
+        <v>23</v>
+      </c>
+      <c r="E19" s="124">
         <v>2018</v>
       </c>
-      <c r="F3" s="96" t="s">
+      <c r="F19" s="87" t="s">
+        <v>537</v>
+      </c>
+      <c r="G19" s="87" t="s">
         <v>63</v>
       </c>
-      <c r="G3" s="96" t="s">
-        <v>60</v>
-      </c>
-      <c r="H3" s="96"/>
-      <c r="I3" s="99" t="s">
-        <v>60</v>
-      </c>
-      <c r="J3" s="109" t="s">
-        <v>565</v>
-      </c>
-      <c r="K3" s="100">
-        <v>7</v>
-      </c>
-      <c r="L3" s="90">
-        <v>6</v>
-      </c>
-      <c r="M3" s="90">
-        <v>4</v>
-      </c>
-      <c r="N3" s="90">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:45" s="97" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="96" t="s">
+      <c r="H19" s="87"/>
+      <c r="I19" s="125"/>
+      <c r="J19" s="125"/>
+      <c r="K19" s="87"/>
+      <c r="L19" s="87"/>
+      <c r="M19" s="87"/>
+      <c r="N19" s="87"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A20" s="130" t="s">
         <v>539</v>
       </c>
-      <c r="B4" s="96" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="96" t="s">
-        <v>32</v>
-      </c>
-      <c r="D4" s="102" t="s">
-        <v>33</v>
-      </c>
-      <c r="E4" s="88">
+      <c r="B20" s="87" t="s">
+        <v>566</v>
+      </c>
+      <c r="C20" s="87" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20" s="87" t="s">
+        <v>29</v>
+      </c>
+      <c r="E20" s="124">
         <v>2018</v>
       </c>
-      <c r="F4" s="96" t="s">
+      <c r="F20" s="87" t="s">
+        <v>537</v>
+      </c>
+      <c r="G20" s="87" t="s">
         <v>63</v>
       </c>
-      <c r="G4" s="96" t="s">
-        <v>60</v>
-      </c>
-      <c r="H4" s="96"/>
-      <c r="I4" s="99" t="s">
-        <v>60</v>
-      </c>
-      <c r="J4" s="111" t="s">
+      <c r="H20" s="87"/>
+      <c r="I20" s="125"/>
+      <c r="J20" s="125"/>
+      <c r="K20" s="87"/>
+      <c r="L20" s="87"/>
+      <c r="M20" s="87"/>
+      <c r="N20" s="87"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A21" s="130" t="s">
+        <v>539</v>
+      </c>
+      <c r="B21" s="87" t="s">
         <v>566</v>
       </c>
-      <c r="K4" s="100">
-        <v>7</v>
-      </c>
-      <c r="L4" s="90">
-        <v>6</v>
-      </c>
-      <c r="M4" s="90">
-        <v>3</v>
-      </c>
-      <c r="N4" s="90">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:45" s="97" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="96" t="s">
+      <c r="C21" s="87" t="s">
+        <v>30</v>
+      </c>
+      <c r="D21" s="87" t="s">
+        <v>31</v>
+      </c>
+      <c r="E21" s="124">
+        <v>2018</v>
+      </c>
+      <c r="F21" s="87" t="s">
+        <v>537</v>
+      </c>
+      <c r="G21" s="87" t="s">
+        <v>63</v>
+      </c>
+      <c r="H21" s="87"/>
+      <c r="I21" s="125"/>
+      <c r="J21" s="125"/>
+      <c r="K21" s="87"/>
+      <c r="L21" s="87"/>
+      <c r="M21" s="87"/>
+      <c r="N21" s="87"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A22" s="130" t="s">
         <v>539</v>
       </c>
-      <c r="B5" s="96" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="96" t="s">
-        <v>40</v>
-      </c>
-      <c r="D5" s="102" t="s">
-        <v>41</v>
-      </c>
-      <c r="E5" s="88">
-        <v>2018</v>
-      </c>
-      <c r="F5" s="96" t="s">
+      <c r="B22" s="87" t="s">
+        <v>566</v>
+      </c>
+      <c r="C22" s="87" t="s">
+        <v>46</v>
+      </c>
+      <c r="D22" s="87" t="s">
+        <v>47</v>
+      </c>
+      <c r="E22" s="124">
+        <v>2017</v>
+      </c>
+      <c r="F22" s="87" t="s">
+        <v>537</v>
+      </c>
+      <c r="G22" s="87" t="s">
         <v>63</v>
       </c>
-      <c r="G5" s="96" t="s">
-        <v>60</v>
-      </c>
-      <c r="H5" s="98" t="s">
-        <v>553</v>
-      </c>
-      <c r="I5" s="99" t="s">
-        <v>60</v>
-      </c>
-      <c r="J5" s="109" t="s">
-        <v>565</v>
-      </c>
-      <c r="K5" s="100">
-        <v>6</v>
-      </c>
-      <c r="L5" s="90">
-        <v>6</v>
-      </c>
-      <c r="M5" s="90">
-        <v>3</v>
-      </c>
-      <c r="N5" s="90">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:45" s="97" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="96" t="s">
+      <c r="H22" s="87"/>
+      <c r="I22" s="125"/>
+      <c r="J22" s="125"/>
+      <c r="K22" s="87"/>
+      <c r="L22" s="87"/>
+      <c r="M22" s="87"/>
+      <c r="N22" s="87"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A23" s="130" t="s">
         <v>539</v>
       </c>
-      <c r="B6" s="96" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="96" t="s">
-        <v>44</v>
-      </c>
-      <c r="D6" s="102" t="s">
-        <v>45</v>
-      </c>
-      <c r="E6" s="88">
-        <v>2017</v>
-      </c>
-      <c r="F6" s="96" t="s">
-        <v>560</v>
-      </c>
-      <c r="G6" s="96" t="s">
-        <v>62</v>
-      </c>
-      <c r="H6" s="96"/>
-      <c r="I6" s="99" t="s">
-        <v>60</v>
-      </c>
-      <c r="J6" s="109" t="s">
-        <v>565</v>
-      </c>
-      <c r="K6" s="66">
-        <v>6</v>
-      </c>
-      <c r="L6" s="89">
-        <v>6</v>
-      </c>
-      <c r="M6" s="89">
-        <v>4</v>
-      </c>
-      <c r="N6" s="89">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:45" s="97" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="96" t="s">
-        <v>539</v>
-      </c>
-      <c r="B7" s="96" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="96" t="s">
-        <v>54</v>
-      </c>
-      <c r="D7" s="102" t="s">
-        <v>55</v>
-      </c>
-      <c r="E7" s="88">
-        <v>2016</v>
-      </c>
-      <c r="F7" s="96" t="s">
+      <c r="B23" s="87" t="s">
+        <v>566</v>
+      </c>
+      <c r="C23" s="87" t="s">
+        <v>58</v>
+      </c>
+      <c r="D23" s="87" t="s">
+        <v>59</v>
+      </c>
+      <c r="E23" s="124">
+        <v>2019</v>
+      </c>
+      <c r="F23" s="87" t="s">
+        <v>537</v>
+      </c>
+      <c r="G23" s="87" t="s">
         <v>63</v>
       </c>
-      <c r="G7" s="96" t="s">
-        <v>61</v>
-      </c>
-      <c r="H7" s="96"/>
-      <c r="I7" s="99" t="s">
-        <v>60</v>
-      </c>
-      <c r="J7" s="109" t="s">
-        <v>565</v>
-      </c>
-      <c r="K7" s="100">
-        <v>7</v>
-      </c>
-      <c r="L7" s="90">
-        <v>7</v>
-      </c>
-      <c r="M7" s="90">
-        <v>2</v>
-      </c>
-      <c r="N7" s="90">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:45" s="97" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="96" t="s">
-        <v>539</v>
-      </c>
-      <c r="B8" s="96" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="96" t="s">
-        <v>56</v>
-      </c>
-      <c r="D8" s="102" t="s">
-        <v>57</v>
-      </c>
-      <c r="E8" s="88">
-        <v>2018</v>
-      </c>
-      <c r="F8" s="96" t="s">
-        <v>63</v>
-      </c>
-      <c r="G8" s="96" t="s">
-        <v>60</v>
-      </c>
-      <c r="H8" s="96"/>
-      <c r="I8" s="99" t="s">
-        <v>60</v>
-      </c>
-      <c r="J8" s="109" t="s">
-        <v>565</v>
-      </c>
-      <c r="K8" s="100">
-        <v>7</v>
-      </c>
-      <c r="L8" s="90">
-        <v>7</v>
-      </c>
-      <c r="M8" s="90">
-        <v>2</v>
-      </c>
-      <c r="N8" s="90">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:45" s="104" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="97" t="s">
-        <v>556</v>
-      </c>
-      <c r="B9" s="113" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="113" t="s">
-        <v>363</v>
-      </c>
-      <c r="D9" s="114" t="s">
-        <v>364</v>
-      </c>
-      <c r="E9" s="115">
-        <v>2016</v>
-      </c>
-      <c r="F9" s="113" t="s">
-        <v>63</v>
-      </c>
-      <c r="G9" s="113" t="s">
-        <v>60</v>
-      </c>
-      <c r="H9" s="113"/>
-      <c r="I9" s="116" t="s">
-        <v>63</v>
-      </c>
-      <c r="J9" s="116"/>
-      <c r="K9" s="96"/>
-      <c r="L9" s="96"/>
-      <c r="M9" s="96"/>
-      <c r="N9" s="96"/>
-      <c r="O9" s="97"/>
-      <c r="P9" s="97"/>
-      <c r="Q9" s="97"/>
-      <c r="R9" s="97"/>
-      <c r="S9" s="97"/>
-      <c r="T9" s="97"/>
-      <c r="U9" s="97"/>
-      <c r="V9" s="97"/>
-      <c r="W9" s="97"/>
-      <c r="X9" s="97"/>
-      <c r="Y9" s="97"/>
-      <c r="Z9" s="97"/>
-      <c r="AA9" s="97"/>
-      <c r="AB9" s="97"/>
-      <c r="AC9" s="97"/>
-      <c r="AD9" s="97"/>
-      <c r="AE9" s="97"/>
-      <c r="AF9" s="97"/>
-      <c r="AG9" s="97"/>
-      <c r="AH9" s="97"/>
-      <c r="AI9" s="97"/>
-      <c r="AJ9" s="97"/>
-      <c r="AK9" s="97"/>
-      <c r="AL9" s="97"/>
-      <c r="AM9" s="97"/>
-      <c r="AN9" s="97"/>
-      <c r="AO9" s="97"/>
-      <c r="AP9" s="97"/>
-      <c r="AQ9" s="97"/>
-      <c r="AR9" s="97"/>
-      <c r="AS9" s="97"/>
-    </row>
-    <row r="10" spans="1:45" s="105" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="97" t="s">
-        <v>538</v>
-      </c>
-      <c r="B10" s="113" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" s="113" t="s">
-        <v>79</v>
-      </c>
-      <c r="D10" s="113" t="s">
-        <v>80</v>
-      </c>
-      <c r="E10" s="115">
-        <v>2017</v>
-      </c>
-      <c r="F10" s="113" t="s">
-        <v>63</v>
-      </c>
-      <c r="G10" s="113" t="s">
-        <v>60</v>
-      </c>
-      <c r="H10" s="113"/>
-      <c r="I10" s="116" t="s">
-        <v>63</v>
-      </c>
-      <c r="J10" s="116"/>
-      <c r="K10" s="96"/>
-      <c r="L10" s="96"/>
-      <c r="M10" s="96"/>
-      <c r="N10" s="96"/>
-      <c r="O10" s="96"/>
-      <c r="P10" s="96"/>
-      <c r="Q10" s="96"/>
-      <c r="R10" s="96"/>
-      <c r="S10" s="96"/>
-      <c r="T10" s="96"/>
-      <c r="U10" s="96"/>
-      <c r="V10" s="96"/>
-      <c r="W10" s="96"/>
-      <c r="X10" s="96"/>
-      <c r="Y10" s="96"/>
-      <c r="Z10" s="96"/>
-      <c r="AA10" s="96"/>
-      <c r="AB10" s="96"/>
-      <c r="AC10" s="96"/>
-      <c r="AD10" s="96"/>
-      <c r="AE10" s="96"/>
-      <c r="AF10" s="96"/>
-      <c r="AG10" s="96"/>
-      <c r="AH10" s="96"/>
-      <c r="AI10" s="96"/>
-      <c r="AJ10" s="96"/>
-      <c r="AK10" s="96"/>
-      <c r="AL10" s="96"/>
-      <c r="AM10" s="96"/>
-      <c r="AN10" s="96"/>
-      <c r="AO10" s="96"/>
-      <c r="AP10" s="96"/>
-      <c r="AQ10" s="96"/>
-      <c r="AR10" s="96"/>
-      <c r="AS10" s="96"/>
-    </row>
-    <row r="11" spans="1:45" s="105" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="104" t="s">
-        <v>538</v>
-      </c>
-      <c r="B11" s="104" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" s="104" t="s">
-        <v>235</v>
-      </c>
-      <c r="D11" s="112" t="s">
-        <v>236</v>
-      </c>
-      <c r="E11" s="50">
-        <v>2017</v>
-      </c>
-      <c r="F11" s="104" t="s">
-        <v>63</v>
-      </c>
-      <c r="G11" s="104" t="s">
-        <v>60</v>
-      </c>
-      <c r="H11" s="104"/>
-      <c r="I11" s="99" t="s">
-        <v>60</v>
-      </c>
-      <c r="J11" s="109" t="s">
-        <v>565</v>
-      </c>
-      <c r="K11" s="110">
-        <v>6</v>
-      </c>
-      <c r="L11" s="85">
-        <v>6</v>
-      </c>
-      <c r="M11" s="85">
-        <v>3</v>
-      </c>
-      <c r="N11" s="85">
-        <v>4</v>
-      </c>
-      <c r="O11" s="96"/>
-      <c r="P11" s="96"/>
-      <c r="Q11" s="96"/>
-      <c r="R11" s="96"/>
-      <c r="S11" s="96"/>
-      <c r="T11" s="96"/>
-      <c r="U11" s="96"/>
-      <c r="V11" s="96"/>
-      <c r="W11" s="96"/>
-      <c r="X11" s="96"/>
-      <c r="Y11" s="96"/>
-      <c r="Z11" s="96"/>
-      <c r="AA11" s="96"/>
-      <c r="AB11" s="96"/>
-      <c r="AC11" s="96"/>
-      <c r="AD11" s="96"/>
-      <c r="AE11" s="96"/>
-      <c r="AF11" s="96"/>
-      <c r="AG11" s="96"/>
-      <c r="AH11" s="96"/>
-      <c r="AI11" s="96"/>
-      <c r="AJ11" s="96"/>
-      <c r="AK11" s="96"/>
-      <c r="AL11" s="96"/>
-      <c r="AM11" s="96"/>
-      <c r="AN11" s="96"/>
-      <c r="AO11" s="96"/>
-      <c r="AP11" s="96"/>
-      <c r="AQ11" s="96"/>
-      <c r="AR11" s="96"/>
-      <c r="AS11" s="96"/>
-    </row>
-    <row r="12" spans="1:45" s="106" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="104" t="s">
-        <v>538</v>
-      </c>
-      <c r="B12" s="104" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" s="104" t="s">
-        <v>249</v>
-      </c>
-      <c r="D12" s="112" t="s">
-        <v>250</v>
-      </c>
-      <c r="E12" s="50">
-        <v>2017</v>
-      </c>
-      <c r="F12" s="104" t="s">
-        <v>63</v>
-      </c>
-      <c r="G12" s="104" t="s">
-        <v>60</v>
-      </c>
-      <c r="H12" s="104"/>
-      <c r="I12" s="99" t="s">
-        <v>60</v>
-      </c>
-      <c r="J12" s="109" t="s">
-        <v>565</v>
-      </c>
-      <c r="K12" s="110">
-        <v>7</v>
-      </c>
-      <c r="L12" s="85">
-        <v>6</v>
-      </c>
-      <c r="M12" s="85">
-        <v>3</v>
-      </c>
-      <c r="N12" s="85">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:45" s="106" customFormat="1" ht="15.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="104" t="s">
-        <v>538</v>
-      </c>
-      <c r="B13" s="104" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" s="104" t="s">
-        <v>301</v>
-      </c>
-      <c r="D13" s="112" t="s">
-        <v>302</v>
-      </c>
-      <c r="E13" s="50">
-        <v>2017</v>
-      </c>
-      <c r="F13" s="104" t="s">
-        <v>63</v>
-      </c>
-      <c r="G13" s="104" t="s">
-        <v>60</v>
-      </c>
-      <c r="H13" s="104"/>
-      <c r="I13" s="99" t="s">
-        <v>60</v>
-      </c>
-      <c r="J13" s="109" t="s">
-        <v>565</v>
-      </c>
-      <c r="K13" s="110">
-        <v>6</v>
-      </c>
-      <c r="L13" s="85">
-        <v>7</v>
-      </c>
-      <c r="M13" s="85">
-        <v>3</v>
-      </c>
-      <c r="N13" s="85">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:45" s="106" customFormat="1" ht="15.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="104" t="s">
-        <v>538</v>
-      </c>
-      <c r="B14" s="104" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" s="104" t="s">
-        <v>355</v>
-      </c>
-      <c r="D14" s="112" t="s">
-        <v>356</v>
-      </c>
-      <c r="E14" s="50">
-        <v>2018</v>
-      </c>
-      <c r="F14" s="104" t="s">
-        <v>63</v>
-      </c>
-      <c r="G14" s="104" t="s">
-        <v>60</v>
-      </c>
-      <c r="H14" s="104"/>
-      <c r="I14" s="99" t="s">
-        <v>60</v>
-      </c>
-      <c r="J14" s="111" t="s">
-        <v>566</v>
-      </c>
-      <c r="K14" s="110">
-        <v>5</v>
-      </c>
-      <c r="L14" s="85">
-        <v>5</v>
-      </c>
-      <c r="M14" s="85">
-        <v>3</v>
-      </c>
-      <c r="N14" s="85">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:45" s="106" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="104" t="s">
-        <v>538</v>
-      </c>
-      <c r="B15" s="104" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" s="104" t="s">
-        <v>369</v>
-      </c>
-      <c r="D15" s="112" t="s">
-        <v>370</v>
-      </c>
-      <c r="E15" s="50">
-        <v>2018</v>
-      </c>
-      <c r="F15" s="104" t="s">
-        <v>63</v>
-      </c>
-      <c r="G15" s="104" t="s">
-        <v>60</v>
-      </c>
-      <c r="H15" s="104"/>
-      <c r="I15" s="99" t="s">
-        <v>60</v>
-      </c>
-      <c r="J15" s="111" t="s">
-        <v>566</v>
-      </c>
-      <c r="K15" s="110">
-        <v>6</v>
-      </c>
-      <c r="L15" s="85">
-        <v>6</v>
-      </c>
-      <c r="M15" s="85">
-        <v>3</v>
-      </c>
-      <c r="N15" s="85">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:45" s="96" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="104" t="s">
-        <v>538</v>
-      </c>
-      <c r="B16" s="104" t="s">
-        <v>5</v>
-      </c>
-      <c r="C16" s="104" t="s">
-        <v>445</v>
-      </c>
-      <c r="D16" s="112" t="s">
-        <v>446</v>
-      </c>
-      <c r="E16" s="50">
-        <v>2017</v>
-      </c>
-      <c r="F16" s="104" t="s">
-        <v>63</v>
-      </c>
-      <c r="G16" s="104" t="s">
-        <v>60</v>
-      </c>
-      <c r="H16" s="104"/>
-      <c r="I16" s="99" t="s">
-        <v>60</v>
-      </c>
-      <c r="J16" s="111" t="s">
-        <v>566</v>
-      </c>
-      <c r="K16" s="110">
-        <v>7</v>
-      </c>
-      <c r="L16" s="85">
-        <v>4</v>
-      </c>
-      <c r="M16" s="85">
-        <v>5</v>
-      </c>
-      <c r="N16" s="85">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" s="96" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="96" t="s">
-        <v>539</v>
-      </c>
-      <c r="B17" s="96" t="s">
-        <v>8</v>
-      </c>
-      <c r="C17" s="96" t="s">
-        <v>14</v>
-      </c>
-      <c r="D17" s="101" t="s">
-        <v>15</v>
-      </c>
-      <c r="E17" s="88">
-        <v>2015</v>
-      </c>
-      <c r="F17" s="96" t="s">
-        <v>63</v>
-      </c>
-      <c r="G17" s="96" t="s">
-        <v>66</v>
-      </c>
-      <c r="H17" s="103"/>
-      <c r="I17" s="99" t="s">
-        <v>60</v>
-      </c>
-      <c r="J17" s="99"/>
-      <c r="K17" s="100">
-        <v>6</v>
-      </c>
-      <c r="L17" s="90">
-        <v>6</v>
-      </c>
-      <c r="M17" s="90">
-        <v>4</v>
-      </c>
-      <c r="N17" s="90">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" s="106" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="96" t="s">
-        <v>539</v>
-      </c>
-      <c r="B18" s="96" t="s">
-        <v>8</v>
-      </c>
-      <c r="C18" s="96" t="s">
-        <v>20</v>
-      </c>
-      <c r="D18" s="101" t="s">
-        <v>21</v>
-      </c>
-      <c r="E18" s="88">
-        <v>2016</v>
-      </c>
-      <c r="F18" s="96" t="s">
-        <v>63</v>
-      </c>
-      <c r="G18" s="96" t="s">
-        <v>66</v>
-      </c>
-      <c r="H18" s="103"/>
-      <c r="I18" s="99" t="s">
-        <v>60</v>
-      </c>
-      <c r="J18" s="99"/>
-      <c r="K18" s="100">
-        <v>7</v>
-      </c>
-      <c r="L18" s="90">
-        <v>6</v>
-      </c>
-      <c r="M18" s="90">
-        <v>4</v>
-      </c>
-      <c r="N18" s="90">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A19" s="106" t="s">
-        <v>539</v>
-      </c>
-      <c r="B19" s="106" t="s">
-        <v>568</v>
-      </c>
-      <c r="C19" s="106" t="s">
-        <v>22</v>
-      </c>
-      <c r="D19" s="107" t="s">
-        <v>23</v>
-      </c>
-      <c r="E19" s="87">
-        <v>2018</v>
-      </c>
-      <c r="F19" s="106" t="s">
-        <v>537</v>
-      </c>
-      <c r="G19" s="106" t="s">
-        <v>63</v>
-      </c>
-      <c r="H19" s="106"/>
-      <c r="I19" s="108"/>
-      <c r="J19" s="108"/>
-      <c r="K19" s="106"/>
-      <c r="L19" s="106"/>
-      <c r="M19" s="106"/>
-      <c r="N19" s="106"/>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A20" s="106" t="s">
-        <v>539</v>
-      </c>
-      <c r="B20" s="106" t="s">
-        <v>568</v>
-      </c>
-      <c r="C20" s="106" t="s">
-        <v>28</v>
-      </c>
-      <c r="D20" s="107" t="s">
-        <v>29</v>
-      </c>
-      <c r="E20" s="87">
-        <v>2018</v>
-      </c>
-      <c r="F20" s="106" t="s">
-        <v>537</v>
-      </c>
-      <c r="G20" s="106" t="s">
-        <v>63</v>
-      </c>
-      <c r="H20" s="106"/>
-      <c r="I20" s="108"/>
-      <c r="J20" s="108"/>
-      <c r="K20" s="106"/>
-      <c r="L20" s="106"/>
-      <c r="M20" s="106"/>
-      <c r="N20" s="106"/>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A21" s="106" t="s">
-        <v>539</v>
-      </c>
-      <c r="B21" s="106" t="s">
-        <v>568</v>
-      </c>
-      <c r="C21" s="106" t="s">
-        <v>30</v>
-      </c>
-      <c r="D21" s="107" t="s">
-        <v>31</v>
-      </c>
-      <c r="E21" s="87">
-        <v>2018</v>
-      </c>
-      <c r="F21" s="106" t="s">
-        <v>537</v>
-      </c>
-      <c r="G21" s="106" t="s">
-        <v>63</v>
-      </c>
-      <c r="H21" s="106"/>
-      <c r="I21" s="108"/>
-      <c r="J21" s="108"/>
-      <c r="K21" s="106"/>
-      <c r="L21" s="106"/>
-      <c r="M21" s="106"/>
-      <c r="N21" s="106"/>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A22" s="106" t="s">
-        <v>539</v>
-      </c>
-      <c r="B22" s="106" t="s">
-        <v>568</v>
-      </c>
-      <c r="C22" s="106" t="s">
-        <v>46</v>
-      </c>
-      <c r="D22" s="106" t="s">
-        <v>47</v>
-      </c>
-      <c r="E22" s="87">
-        <v>2017</v>
-      </c>
-      <c r="F22" s="106" t="s">
-        <v>537</v>
-      </c>
-      <c r="G22" s="106" t="s">
-        <v>63</v>
-      </c>
-      <c r="H22" s="106"/>
-      <c r="I22" s="108"/>
-      <c r="J22" s="108"/>
-      <c r="K22" s="106"/>
-      <c r="L22" s="106"/>
-      <c r="M22" s="106"/>
-      <c r="N22" s="106"/>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A23" s="106" t="s">
-        <v>539</v>
-      </c>
-      <c r="B23" s="106" t="s">
-        <v>568</v>
-      </c>
-      <c r="C23" s="106" t="s">
-        <v>58</v>
-      </c>
-      <c r="D23" s="106" t="s">
-        <v>59</v>
-      </c>
-      <c r="E23" s="87">
-        <v>2019</v>
-      </c>
-      <c r="F23" s="106" t="s">
-        <v>537</v>
-      </c>
-      <c r="G23" s="106" t="s">
-        <v>63</v>
-      </c>
-      <c r="H23" s="106"/>
-      <c r="I23" s="108"/>
-      <c r="J23" s="108"/>
-      <c r="K23" s="106"/>
-      <c r="L23" s="106"/>
-      <c r="M23" s="106"/>
-      <c r="N23" s="106"/>
+      <c r="H23" s="87"/>
+      <c r="I23" s="125"/>
+      <c r="J23" s="125"/>
+      <c r="K23" s="87"/>
+      <c r="L23" s="87"/>
+      <c r="M23" s="87"/>
+      <c r="N23" s="87"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:N23" xr:uid="{48964EBD-FBE9-433B-8AE9-6BDEB6875024}">
@@ -3775,7 +3722,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="E1" s="66" t="s">
         <v>72</v>
@@ -3790,7 +3737,7 @@
         <v>71</v>
       </c>
       <c r="I1" s="72" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>73</v>
@@ -88717,7 +88664,7 @@
   <dimension ref="B1:M5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -88730,35 +88677,35 @@
   <sheetData>
     <row r="1" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="2:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="117" t="s">
+      <c r="B2" s="88" t="s">
         <v>510</v>
       </c>
-      <c r="C2" s="119" t="s">
+      <c r="C2" s="90" t="s">
         <v>509</v>
       </c>
-      <c r="D2" s="120" t="s">
+      <c r="D2" s="91" t="s">
         <v>508</v>
       </c>
-      <c r="E2" s="121" t="s">
+      <c r="E2" s="92" t="s">
         <v>507</v>
       </c>
-      <c r="F2" s="122"/>
-      <c r="G2" s="123"/>
-      <c r="H2" s="117" t="s">
+      <c r="F2" s="93"/>
+      <c r="G2" s="94"/>
+      <c r="H2" s="88" t="s">
         <v>506</v>
       </c>
-      <c r="I2" s="119"/>
-      <c r="J2" s="120"/>
-      <c r="K2" s="124" t="s">
+      <c r="I2" s="90"/>
+      <c r="J2" s="91"/>
+      <c r="K2" s="95" t="s">
         <v>505</v>
       </c>
-      <c r="L2" s="125"/>
-      <c r="M2" s="126"/>
+      <c r="L2" s="96"/>
+      <c r="M2" s="97"/>
     </row>
     <row r="3" spans="2:13" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B3" s="118"/>
-      <c r="C3" s="128"/>
-      <c r="D3" s="127"/>
+      <c r="B3" s="89"/>
+      <c r="C3" s="99"/>
+      <c r="D3" s="98"/>
       <c r="E3" s="38" t="s">
         <v>504</v>
       </c>
@@ -88980,7 +88927,7 @@
     </row>
     <row r="5" spans="1:10" s="53" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="53" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="C5" s="49" t="s">
         <v>6</v>
@@ -89009,7 +88956,7 @@
     </row>
     <row r="6" spans="1:10" s="53" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="53" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="C6" s="49" t="s">
         <v>140</v>
@@ -89469,7 +89416,7 @@
   <sheetData>
     <row r="1" spans="1:14" s="2" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A1" s="77" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
@@ -89490,13 +89437,13 @@
         <v>67</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="K1" s="66" t="s">
         <v>72</v>
@@ -89513,7 +89460,7 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="78" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>5</v>
@@ -89538,7 +89485,7 @@
     </row>
     <row r="3" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="78" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>5</v>
@@ -89563,7 +89510,7 @@
     </row>
     <row r="4" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="78" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>5</v>
@@ -89588,7 +89535,7 @@
     </row>
     <row r="5" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="78" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>5</v>
@@ -89613,7 +89560,7 @@
     </row>
     <row r="6" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="78" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>5</v>
@@ -89638,7 +89585,7 @@
     </row>
     <row r="7" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="78" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>5</v>
@@ -89663,7 +89610,7 @@
     </row>
     <row r="8" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="78" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>5</v>
@@ -89674,7 +89621,7 @@
       <c r="D8" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="E8" s="86">
+      <c r="E8" s="85">
         <v>2018</v>
       </c>
       <c r="F8" s="4" t="s">
@@ -89688,7 +89635,7 @@
     </row>
     <row r="9" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="78" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>5</v>
@@ -89713,7 +89660,7 @@
     </row>
     <row r="10" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="78" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>5</v>
@@ -89738,7 +89685,7 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" s="78" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="B11" t="s">
         <v>8</v>
@@ -89761,7 +89708,7 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" s="78" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="B12" t="s">
         <v>8</v>
@@ -89784,7 +89731,7 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" s="78" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="B13" t="s">
         <v>8</v>
@@ -89807,7 +89754,7 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" s="78" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="B14" t="s">
         <v>8</v>
@@ -89830,7 +89777,7 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" s="78" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="B15" t="s">
         <v>8</v>
@@ -89853,7 +89800,7 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" s="78" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="B16" t="s">
         <v>8</v>
@@ -89876,7 +89823,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="78" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="B17" t="s">
         <v>8</v>

</xml_diff>